<commit_message>
Updated Excel watcher and Docker setup
</commit_message>
<xml_diff>
--- a/src/contacts.xlsx
+++ b/src/contacts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\dataCleansing\data-cleansing-server\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0561A8A-8126-4DB8-B7D1-F314C2862985}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1DCD973-0212-4547-A564-E94EC051BBB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-26910" yWindow="3645" windowWidth="21600" windowHeight="11235" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="45">
   <si>
     <t>agent</t>
   </si>
@@ -154,9 +154,6 @@
   </si>
   <si>
     <t>transport</t>
-  </si>
-  <si>
-    <t>person 1</t>
   </si>
   <si>
     <t>050-9999998</t>
@@ -536,7 +533,7 @@
   <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD11"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -573,7 +570,7 @@
         <v>34</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I1" s="6" t="s">
         <v>38</v>
@@ -587,13 +584,13 @@
         <v>41</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>43</v>
+        <v>15</v>
       </c>
       <c r="D2" s="9" t="s">
         <v>24</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>35</v>
@@ -622,7 +619,7 @@
         <v>25</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>35</v>
@@ -651,7 +648,7 @@
         <v>26</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>35</v>
@@ -680,7 +677,7 @@
         <v>27</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>35</v>
@@ -709,7 +706,7 @@
         <v>28</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>35</v>
@@ -738,7 +735,7 @@
         <v>29</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F7" s="3" t="s">
         <v>35</v>
@@ -767,7 +764,7 @@
         <v>30</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F8" s="3" t="s">
         <v>35</v>
@@ -796,7 +793,7 @@
         <v>31</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F9" s="3" t="s">
         <v>35</v>
@@ -825,7 +822,7 @@
         <v>32</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F10" s="3" t="s">
         <v>35</v>
@@ -854,7 +851,7 @@
         <v>33</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F11" s="3" t="s">
         <v>35</v>

</xml_diff>